<commit_message>
updated cart test cases excel file
</commit_message>
<xml_diff>
--- a/manual-testing/test-cases/Cart_Test_Cases.xlsx
+++ b/manual-testing/test-cases/Cart_Test_Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -133,7 +133,8 @@
   </si>
   <si>
     <t>- Item should disappear from checkout page
-- Cart badge should disappear</t>
+- Cart badge should disappear
+- Checkout button should be disabled</t>
   </si>
   <si>
     <t>TC_CART_REMOVE_02</t>
@@ -171,7 +172,8 @@
   </si>
   <si>
     <t>- Item should disappear from checkout page
-- Cart badge should decrease by 1</t>
+- Cart badge should decrease by 1
+- Checkout button should be available</t>
   </si>
   <si>
     <t>TC_CART_REMOVE_04</t>
@@ -238,6 +240,22 @@
   <si>
     <t>- User should be redirected to products page
 - Added products should still be in cart</t>
+  </si>
+  <si>
+    <t>TC_CART_PAGE_04</t>
+  </si>
+  <si>
+    <t>Open cart page when cart is empty</t>
+  </si>
+  <si>
+    <t>User is logged in with a valid account
+User is on the Products page
+Cart is empty</t>
+  </si>
+  <si>
+    <t>- User should be redirected to cart page
+- No items should be visible
+- Checkout button should be disabled</t>
   </si>
 </sst>
 </file>
@@ -875,15 +893,31 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="A13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9"/>
+      <c r="H13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="8"/>
@@ -10760,10 +10794,10 @@
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H13">
       <formula1>"Low,Medium,High"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I13">
       <formula1>"Not Run,Pass,Fail,In Progress,Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>